<commit_message>
added file upload options
</commit_message>
<xml_diff>
--- a/input/Commands/CommonCommandList.xlsx
+++ b/input/Commands/CommonCommandList.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52da370e166b9526/Development/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A659380-3C2A-481E-B02E-74682BF83FA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="11790" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14340" windowHeight="10200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -19,17 +20,22 @@
   <definedNames>
     <definedName name="Project_Name">Notes!$B$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="96">
   <si>
     <t>Name of project</t>
   </si>
@@ -311,12 +317,18 @@
   </si>
   <si>
     <t>sudo systemctl status mssql-server</t>
+  </si>
+  <si>
+    <t>Edit share drive mount file</t>
+  </si>
+  <si>
+    <t>sudo nano /etc/fstab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -670,7 +682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -710,7 +722,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:F322"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4043,18 +4055,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F12" r:id="rId1"/>
+    <hyperlink ref="F12" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F322"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B3:F323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4098,7 +4110,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
-        <f t="shared" ref="B5:C68" si="0">ROW()-3</f>
+        <f t="shared" ref="B5:B68" si="0">ROW()-3</f>
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -4141,8 +4153,12 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
@@ -4151,9 +4167,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -4164,11 +4178,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>77</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -4176,13 +4189,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>75</v>
+      <c r="C11" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="3"/>
+        <v>77</v>
+      </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -4191,12 +4203,12 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -4204,8 +4216,12 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
     </row>
@@ -4214,11 +4230,9 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -4227,11 +4241,9 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>81</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
@@ -4241,10 +4253,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -4255,10 +4267,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -4269,10 +4281,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -4282,8 +4294,12 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
@@ -4292,9 +4308,8 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
@@ -4304,10 +4319,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -4318,10 +4330,10 @@
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -4331,8 +4343,12 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
@@ -4441,9 +4457,9 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="4"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -4451,9 +4467,9 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="4"/>
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -7318,7 +7334,13 @@
       <c r="E322" s="3"/>
       <c r="F322" s="3"/>
     </row>
+    <row r="323" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C323" s="3"/>
+      <c r="D323" s="3"/>
+      <c r="E323" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>